<commit_message>
Endret navn på barnehagene til relevante i Drammen Kommune
</commit_message>
<xml_diff>
--- a/barnehage/kgdata.xlsx
+++ b/barnehage/kgdata.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sunshine Preschool</t>
+          <t>Amicus barnehage</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -532,7 +532,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Happy Days Nursery</t>
+          <t>Aronsløkka barnehage</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -551,7 +551,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>123 Learning Center</t>
+          <t>Bacheparken barnehage</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -570,7 +570,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ABC Kindergarten</t>
+          <t>Blåbærtoppen barnehage</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -589,7 +589,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Tiny Tots Academy</t>
+          <t>Dalegårdsveien barnehage</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -608,11 +608,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Giggles and Grins Childcare</t>
+          <t>Ekornheia barnehage</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -627,7 +627,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Playful Pals Daycare</t>
+          <t>Eplehagan barnehage</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -679,7 +679,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -766,6 +766,11 @@
       <c r="P1" s="1" t="inlineStr">
         <is>
           <t>beslutning</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>fortrinnsrett</t>
         </is>
       </c>
     </row>
@@ -785,17 +790,22 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Ola Nordmann</t>
+          <t>Haakon Halvorsen</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Sunshine Preschool</t>
+          <t>Amicus barnehage</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
           <t>TILBUD</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Nei</t>
         </is>
       </c>
     </row>
@@ -820,12 +830,17 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Giggles and Grins Childcare</t>
+          <t>Amicus barnehage</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>AVSLAG: Ingen ledige plasser.</t>
+          <t>TILBUD</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Ja</t>
         </is>
       </c>
     </row>
@@ -850,14 +865,571 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Sunshine Preschool</t>
+          <t>Blåbærtoppen barnehage</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
+          <t>AVSLAG: Ingen ledige plasser.</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Haakon Halvorsen</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Blåbærtoppen barnehage</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>AVSLAG: Ingen ledige plasser.</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Haakon Halvorsen</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Blåbærtoppen barnehage</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>AVSLAG: Ingen ledige plasser.</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Haakon Halvorsen</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Amicus barnehage</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
           <t>TILBUD</t>
         </is>
       </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Haakon Halvorsen</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Amicus barnehage</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>TILBUD</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Haakon Halvorsen</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Eplehagan barnehage</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>TILBUD</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Haakon Halvorsen</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Eplehagan barnehage</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>TILBUD</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Ola Nordmann</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Blåbærtoppen barnehage</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>AVSLAG: Barnet er under ett år.</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Ola Nordmann</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Blåbærtoppen barnehage</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>AVSLAG: Ingen ledige plasser.</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Ola Nordmann</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Amicus barnehage</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>TILBUD</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Ola Nordmann</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Amicus barnehage</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>TILBUD</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Ola Nordmann</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Amicus barnehage</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>TILBUD</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Ola Nordmann</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Amicus barnehage</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>TILBUD</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Ola Nordmann</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Amicus barnehage</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>TILBUD</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Ola Nordmann</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Amicus barnehage</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>TILBUD</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Nei</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Ola Nordmann</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Dalegårdsveien barnehage</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>TILBUD</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Ola Nordmann</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Dalegårdsveien barnehage</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>AVSLAG: Barnet er under ett år.</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fjernet et unødvendig fil
</commit_message>
<xml_diff>
--- a/barnehage/kgdata.xlsx
+++ b/barnehage/kgdata.xlsx
@@ -679,7 +679,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1431,6 +1431,37 @@
       </c>
       <c r="Q20" t="inlineStr"/>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Ola Nordmann</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Amicus barnehage</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>TILBUD</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>